<commit_message>
Adding new attribute during import for MysqlRepository
</commit_message>
<xml_diff>
--- a/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="980" windowWidth="31340" windowHeight="18980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="129">
   <si>
     <t>text</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>rangeMax</t>
+  </si>
+  <si>
+    <t>lookupAttribute</t>
   </si>
 </sst>
 </file>
@@ -774,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
@@ -4713,10 +4716,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4729,7 +4732,7 @@
     <col min="7" max="7" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>99</v>
       </c>
@@ -4757,8 +4760,11 @@
       <c r="I1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4774,8 +4780,11 @@
       <c r="F2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -4792,7 +4801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -4809,7 +4818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -4826,7 +4835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -4846,7 +4855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -4866,7 +4875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -4883,7 +4892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -4900,7 +4909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -4917,7 +4926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -4934,7 +4943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -4951,7 +4960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -4968,7 +4977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -4985,7 +4994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -5002,7 +5011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Fix int/long/decimal/date/datetime aggregation + update example data
</commit_message>
<xml_diff>
--- a/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -684,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="AK2" sqref="AK2:AK21"/>
     </sheetView>
   </sheetViews>
@@ -4605,8 +4605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4823,6 +4823,9 @@
       <c r="F9" t="b">
         <v>0</v>
       </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -4874,6 +4877,9 @@
       <c r="F12" t="b">
         <v>1</v>
       </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -4891,6 +4897,9 @@
       <c r="F13" t="b">
         <v>0</v>
       </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -4925,6 +4934,9 @@
       <c r="F15" t="b">
         <v>0</v>
       </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -5019,6 +5031,9 @@
       <c r="F20" t="b">
         <v>1</v>
       </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -5036,6 +5051,9 @@
       <c r="F21" t="b">
         <v>0</v>
       </c>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -5193,6 +5211,9 @@
       <c r="I29">
         <v>10</v>
       </c>
+      <c r="M29" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -5215,6 +5236,9 @@
       </c>
       <c r="I30">
         <v>10</v>
+      </c>
+      <c r="M30" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Unique columns in MysqRepository
</commit_message>
<xml_diff>
--- a/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19380" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="137">
   <si>
     <t>text</t>
   </si>
@@ -316,6 +316,123 @@
   </si>
   <si>
     <t>hidden</t>
+  </si>
+  <si>
+    <t>xstring_unique</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>xint_unique</t>
+  </si>
+  <si>
+    <t>str4</t>
+  </si>
+  <si>
+    <t>str5</t>
+  </si>
+  <si>
+    <t>str6</t>
+  </si>
+  <si>
+    <t>str7</t>
+  </si>
+  <si>
+    <t>str8</t>
+  </si>
+  <si>
+    <t>str9</t>
+  </si>
+  <si>
+    <t>str10</t>
+  </si>
+  <si>
+    <t>str11</t>
+  </si>
+  <si>
+    <t>str12</t>
+  </si>
+  <si>
+    <t>str13</t>
+  </si>
+  <si>
+    <t>str14</t>
+  </si>
+  <si>
+    <t>str15</t>
+  </si>
+  <si>
+    <t>str16</t>
+  </si>
+  <si>
+    <t>str17</t>
+  </si>
+  <si>
+    <t>str18</t>
+  </si>
+  <si>
+    <t>str19</t>
+  </si>
+  <si>
+    <t>str20</t>
+  </si>
+  <si>
+    <t>str21</t>
+  </si>
+  <si>
+    <t>str22</t>
+  </si>
+  <si>
+    <t>str23</t>
+  </si>
+  <si>
+    <t>str24</t>
+  </si>
+  <si>
+    <t>str25</t>
+  </si>
+  <si>
+    <t>str26</t>
+  </si>
+  <si>
+    <t>str27</t>
+  </si>
+  <si>
+    <t>str28</t>
+  </si>
+  <si>
+    <t>str29</t>
+  </si>
+  <si>
+    <t>str30</t>
+  </si>
+  <si>
+    <t>str31</t>
+  </si>
+  <si>
+    <t>str32</t>
+  </si>
+  <si>
+    <t>str33</t>
+  </si>
+  <si>
+    <t>str34</t>
+  </si>
+  <si>
+    <t>str35</t>
+  </si>
+  <si>
+    <t>str36</t>
+  </si>
+  <si>
+    <t>str37</t>
+  </si>
+  <si>
+    <t>str38</t>
+  </si>
+  <si>
+    <t>xxref_unique</t>
   </si>
 </sst>
 </file>
@@ -364,9 +481,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -377,11 +496,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -682,37 +803,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK39"/>
+  <dimension ref="A1:AN39"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2:AK21"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AN6" sqref="AN6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="24" customWidth="1"/>
-    <col min="35" max="35" width="23.42578125" customWidth="1"/>
-    <col min="36" max="36" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.5" customWidth="1"/>
+    <col min="36" max="36" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -824,8 +946,17 @@
       <c r="AK1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
       <c r="A2">
         <v>1</v>
       </c>
@@ -937,8 +1068,17 @@
       <c r="AK2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM2">
+        <v>1</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1050,8 +1190,17 @@
       <c r="AK3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM3">
+        <v>2</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1112,8 +1261,17 @@
       <c r="AK4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM4">
+        <v>3</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1225,8 +1383,17 @@
       <c r="AK5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM5">
+        <v>4</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1338,8 +1505,17 @@
       <c r="AK6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM6">
+        <v>5</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1400,8 +1576,14 @@
       <c r="AK7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL7" t="s">
+        <v>103</v>
+      </c>
+      <c r="AM7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1513,8 +1695,14 @@
       <c r="AK8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1626,8 +1814,14 @@
       <c r="AK9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1688,8 +1882,14 @@
       <c r="AK10" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AM10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1801,8 +2001,14 @@
       <c r="AK11" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL11" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1914,8 +2120,14 @@
       <c r="AK12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL12" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1976,8 +2188,14 @@
       <c r="AK13" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL13" t="s">
+        <v>109</v>
+      </c>
+      <c r="AM13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2089,8 +2307,14 @@
       <c r="AK14" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2202,8 +2426,14 @@
       <c r="AK15" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL15" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2264,8 +2494,14 @@
       <c r="AK16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL16" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2326,8 +2562,14 @@
       <c r="AK17" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL17" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2439,8 +2681,14 @@
       <c r="AK18" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL18" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2552,8 +2800,14 @@
       <c r="AK19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL19" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2614,8 +2868,14 @@
       <c r="AK20" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL20" t="s">
+        <v>116</v>
+      </c>
+      <c r="AM20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2727,8 +2987,14 @@
       <c r="AK21" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL21" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2837,8 +3103,14 @@
       <c r="AJ22" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL22" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2896,8 +3168,14 @@
       <c r="AJ23" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL23" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3006,8 +3284,14 @@
       <c r="AJ24" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL24" t="s">
+        <v>120</v>
+      </c>
+      <c r="AM24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3116,8 +3400,14 @@
       <c r="AJ25" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL25" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3175,8 +3465,14 @@
       <c r="AJ26" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL26" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3285,8 +3581,14 @@
       <c r="AJ27" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL27" t="s">
+        <v>123</v>
+      </c>
+      <c r="AM27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3395,8 +3697,14 @@
       <c r="AJ28" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL28" t="s">
+        <v>124</v>
+      </c>
+      <c r="AM28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3454,8 +3762,14 @@
       <c r="AJ29" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL29" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3564,8 +3878,14 @@
       <c r="AJ30" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL30" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3674,8 +3994,14 @@
       <c r="AJ31" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL31" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3733,8 +4059,14 @@
       <c r="AJ32" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AL32" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3843,8 +4175,14 @@
       <c r="AJ33" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AL33" t="s">
+        <v>129</v>
+      </c>
+      <c r="AM33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3953,8 +4291,14 @@
       <c r="AJ34" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AL34" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4012,8 +4356,14 @@
       <c r="AJ35" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AL35" t="s">
+        <v>131</v>
+      </c>
+      <c r="AM35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4071,8 +4421,14 @@
       <c r="AJ36" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AL36" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4181,8 +4537,14 @@
       <c r="AJ37" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AL37" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4291,8 +4653,14 @@
       <c r="AJ38" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AL38" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4349,6 +4717,12 @@
       </c>
       <c r="AJ39" t="s">
         <v>97</v>
+      </c>
+      <c r="AL39" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM39">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -4496,9 +4870,9 @@
       <selection activeCell="A7" sqref="A7:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4506,7 +4880,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4514,7 +4888,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4522,7 +4896,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4530,7 +4904,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -4538,7 +4912,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -4564,13 +4938,13 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -4578,7 +4952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -4586,7 +4960,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -4603,24 +4977,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -4663,8 +5037,11 @@
       <c r="N1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4684,7 +5061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -4707,7 +5084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -4727,7 +5104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -4747,7 +5124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4767,7 +5144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -4787,7 +5164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -4807,7 +5184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4827,7 +5204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -4844,7 +5221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -4861,7 +5238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -4881,7 +5258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -4901,7 +5278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -4918,7 +5295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -4938,7 +5315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -4955,7 +5332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -4978,7 +5355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -4998,7 +5375,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -5015,7 +5392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -5035,7 +5412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -5055,7 +5432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -5072,7 +5449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -5092,7 +5469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -5109,7 +5486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -5132,7 +5509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -5155,7 +5532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -5172,7 +5549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -5189,7 +5566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -5215,7 +5592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -5241,7 +5618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -5264,7 +5641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -5284,7 +5661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -5304,7 +5681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -5321,7 +5698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -5338,7 +5715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -5355,7 +5732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -5378,7 +5755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -5398,7 +5775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -5418,7 +5795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -5436,6 +5813,69 @@
       </c>
       <c r="N40" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="O41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="O42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="O43" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor to new meta data api design
</commit_message>
<xml_diff>
--- a/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
     <sheet name="TypeTestRef" sheetId="2" r:id="rId2"/>
-    <sheet name="entities" sheetId="3" r:id="rId3"/>
-    <sheet name="attributes" sheetId="4" r:id="rId4"/>
+    <sheet name="packages" sheetId="5" r:id="rId3"/>
+    <sheet name="entities" sheetId="3" r:id="rId4"/>
+    <sheet name="attributes" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="141">
   <si>
     <t>text</t>
   </si>
@@ -433,6 +434,18 @@
   </si>
   <si>
     <t>xxref_unique</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Molgenis test package</t>
+  </si>
+  <si>
+    <t>package</t>
   </si>
 </sst>
 </file>
@@ -805,7 +818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView topLeftCell="AG1" workbookViewId="0">
       <selection activeCell="AN7" sqref="AN7"/>
     </sheetView>
   </sheetViews>
@@ -4932,37 +4945,86 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
       <c r="B1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
       <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4975,7 +5037,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O43"/>
   <sheetViews>

</xml_diff>

<commit_message>
Prototype BMB standards registry
</commit_message>
<xml_diff>
--- a/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17740" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="239">
   <si>
     <t>text</t>
   </si>
@@ -452,6 +452,294 @@
   </si>
   <si>
     <t>org</t>
+  </si>
+  <si>
+    <t>pack1</t>
+  </si>
+  <si>
+    <t>pack2</t>
+  </si>
+  <si>
+    <t>pack3</t>
+  </si>
+  <si>
+    <t>pack4</t>
+  </si>
+  <si>
+    <t>pack5</t>
+  </si>
+  <si>
+    <t>pack6</t>
+  </si>
+  <si>
+    <t>pack7</t>
+  </si>
+  <si>
+    <t>pack8</t>
+  </si>
+  <si>
+    <t>pack9</t>
+  </si>
+  <si>
+    <t>pack10</t>
+  </si>
+  <si>
+    <t>pack11</t>
+  </si>
+  <si>
+    <t>pack12</t>
+  </si>
+  <si>
+    <t>pack13</t>
+  </si>
+  <si>
+    <t>pack14</t>
+  </si>
+  <si>
+    <t>pack15</t>
+  </si>
+  <si>
+    <t>pack16</t>
+  </si>
+  <si>
+    <t>pack17</t>
+  </si>
+  <si>
+    <t>pack18</t>
+  </si>
+  <si>
+    <t>pack19</t>
+  </si>
+  <si>
+    <t>pack20</t>
+  </si>
+  <si>
+    <t>pack21</t>
+  </si>
+  <si>
+    <t>pack22</t>
+  </si>
+  <si>
+    <t>pack23</t>
+  </si>
+  <si>
+    <t>pack24</t>
+  </si>
+  <si>
+    <t>pack25</t>
+  </si>
+  <si>
+    <t>pack26</t>
+  </si>
+  <si>
+    <t>pack27</t>
+  </si>
+  <si>
+    <t>pack28</t>
+  </si>
+  <si>
+    <t>pack29</t>
+  </si>
+  <si>
+    <t>pack30</t>
+  </si>
+  <si>
+    <t>pack31</t>
+  </si>
+  <si>
+    <t>pack32</t>
+  </si>
+  <si>
+    <t>pack33</t>
+  </si>
+  <si>
+    <t>pack34</t>
+  </si>
+  <si>
+    <t>pack35</t>
+  </si>
+  <si>
+    <t>pack36</t>
+  </si>
+  <si>
+    <t>pack37</t>
+  </si>
+  <si>
+    <t>pack38</t>
+  </si>
+  <si>
+    <t>pack39</t>
+  </si>
+  <si>
+    <t>pack40</t>
+  </si>
+  <si>
+    <t>pack41</t>
+  </si>
+  <si>
+    <t>pack42</t>
+  </si>
+  <si>
+    <t>pack43</t>
+  </si>
+  <si>
+    <t>pack44</t>
+  </si>
+  <si>
+    <t>pack45</t>
+  </si>
+  <si>
+    <t>pack46</t>
+  </si>
+  <si>
+    <t>pack47</t>
+  </si>
+  <si>
+    <t>pack48</t>
+  </si>
+  <si>
+    <t>pack49</t>
+  </si>
+  <si>
+    <t>pack50</t>
+  </si>
+  <si>
+    <t>pack51</t>
+  </si>
+  <si>
+    <t>pack52</t>
+  </si>
+  <si>
+    <t>pack53</t>
+  </si>
+  <si>
+    <t>pack54</t>
+  </si>
+  <si>
+    <t>pack55</t>
+  </si>
+  <si>
+    <t>pack56</t>
+  </si>
+  <si>
+    <t>pack57</t>
+  </si>
+  <si>
+    <t>pack58</t>
+  </si>
+  <si>
+    <t>pack59</t>
+  </si>
+  <si>
+    <t>pack60</t>
+  </si>
+  <si>
+    <t>pack61</t>
+  </si>
+  <si>
+    <t>pack62</t>
+  </si>
+  <si>
+    <t>pack63</t>
+  </si>
+  <si>
+    <t>pack64</t>
+  </si>
+  <si>
+    <t>pack65</t>
+  </si>
+  <si>
+    <t>pack66</t>
+  </si>
+  <si>
+    <t>pack67</t>
+  </si>
+  <si>
+    <t>pack68</t>
+  </si>
+  <si>
+    <t>pack69</t>
+  </si>
+  <si>
+    <t>pack70</t>
+  </si>
+  <si>
+    <t>pack71</t>
+  </si>
+  <si>
+    <t>pack72</t>
+  </si>
+  <si>
+    <t>pack73</t>
+  </si>
+  <si>
+    <t>pack74</t>
+  </si>
+  <si>
+    <t>pack75</t>
+  </si>
+  <si>
+    <t>pack76</t>
+  </si>
+  <si>
+    <t>pack77</t>
+  </si>
+  <si>
+    <t>pack78</t>
+  </si>
+  <si>
+    <t>pack79</t>
+  </si>
+  <si>
+    <t>pack80</t>
+  </si>
+  <si>
+    <t>pack81</t>
+  </si>
+  <si>
+    <t>pack82</t>
+  </si>
+  <si>
+    <t>pack83</t>
+  </si>
+  <si>
+    <t>pack84</t>
+  </si>
+  <si>
+    <t>pack85</t>
+  </si>
+  <si>
+    <t>pack86</t>
+  </si>
+  <si>
+    <t>pack87</t>
+  </si>
+  <si>
+    <t>pack88</t>
+  </si>
+  <si>
+    <t>pack89</t>
+  </si>
+  <si>
+    <t>pack90</t>
+  </si>
+  <si>
+    <t>pack91</t>
+  </si>
+  <si>
+    <t>pack92</t>
+  </si>
+  <si>
+    <t>pack93</t>
+  </si>
+  <si>
+    <t>pack94</t>
+  </si>
+  <si>
+    <t>pack95</t>
+  </si>
+  <si>
+    <t>pack96</t>
   </si>
 </sst>
 </file>
@@ -828,32 +1116,32 @@
       <selection activeCell="AN7" sqref="AN7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="24" customWidth="1"/>
-    <col min="35" max="35" width="23.5" customWidth="1"/>
-    <col min="36" max="36" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.33203125" customWidth="1"/>
+    <col min="35" max="35" width="23.42578125" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -975,7 +1263,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1097,7 +1385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1219,7 +1507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1290,7 +1578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1412,7 +1700,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1534,7 +1822,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1602,7 +1890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1721,7 +2009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1840,7 +2128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1908,7 +2196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2027,7 +2315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2146,7 +2434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2214,7 +2502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2333,7 +2621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2452,7 +2740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2520,7 +2808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2588,7 +2876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2707,7 +2995,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2826,7 +3114,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2894,7 +3182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3013,7 +3301,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3129,7 +3417,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3194,7 +3482,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3310,7 +3598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3426,7 +3714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3491,7 +3779,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3607,7 +3895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3723,7 +4011,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:39">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3788,7 +4076,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:39">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3904,7 +4192,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:39">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4020,7 +4308,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:39">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4085,7 +4373,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4201,7 +4489,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4317,7 +4605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4382,7 +4670,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4447,7 +4735,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4563,7 +4851,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4679,7 +4967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4889,9 +5177,9 @@
       <selection activeCell="A7" sqref="A7:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4899,7 +5187,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4907,7 +5195,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4915,7 +5203,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4923,7 +5211,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -4931,7 +5219,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -4951,18 +5239,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -4973,7 +5261,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -4984,7 +5272,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -4992,9 +5280,489 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -5015,14 +5783,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5033,7 +5801,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -5044,7 +5812,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -5070,18 +5838,18 @@
       <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5128,7 +5896,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5148,7 +5916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5171,7 +5939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5191,7 +5959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5211,7 +5979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5231,7 +5999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -5251,7 +6019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -5271,7 +6039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -5291,7 +6059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -5308,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -5325,7 +6093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -5345,7 +6113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -5365,7 +6133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -5382,7 +6150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -5402,7 +6170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5419,7 +6187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -5442,7 +6210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -5462,7 +6230,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -5479,7 +6247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -5499,7 +6267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -5519,7 +6287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -5536,7 +6304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -5556,7 +6324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -5573,7 +6341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -5596,7 +6364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -5619,7 +6387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -5636,7 +6404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -5653,7 +6421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -5679,7 +6447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -5705,7 +6473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -5728,7 +6496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -5748,7 +6516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -5768,7 +6536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -5785,7 +6553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -5802,7 +6570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -5819,7 +6587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -5842,7 +6610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -5862,7 +6630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -5882,7 +6650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -5902,7 +6670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -5922,7 +6690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -5942,7 +6710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
revert merge with chao branch
</commit_message>
<xml_diff>
--- a/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16440" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="143">
   <si>
     <t>text</t>
   </si>
@@ -452,294 +452,6 @@
   </si>
   <si>
     <t>org</t>
-  </si>
-  <si>
-    <t>pack1</t>
-  </si>
-  <si>
-    <t>pack2</t>
-  </si>
-  <si>
-    <t>pack3</t>
-  </si>
-  <si>
-    <t>pack4</t>
-  </si>
-  <si>
-    <t>pack5</t>
-  </si>
-  <si>
-    <t>pack6</t>
-  </si>
-  <si>
-    <t>pack7</t>
-  </si>
-  <si>
-    <t>pack8</t>
-  </si>
-  <si>
-    <t>pack9</t>
-  </si>
-  <si>
-    <t>pack10</t>
-  </si>
-  <si>
-    <t>pack11</t>
-  </si>
-  <si>
-    <t>pack12</t>
-  </si>
-  <si>
-    <t>pack13</t>
-  </si>
-  <si>
-    <t>pack14</t>
-  </si>
-  <si>
-    <t>pack15</t>
-  </si>
-  <si>
-    <t>pack16</t>
-  </si>
-  <si>
-    <t>pack17</t>
-  </si>
-  <si>
-    <t>pack18</t>
-  </si>
-  <si>
-    <t>pack19</t>
-  </si>
-  <si>
-    <t>pack20</t>
-  </si>
-  <si>
-    <t>pack21</t>
-  </si>
-  <si>
-    <t>pack22</t>
-  </si>
-  <si>
-    <t>pack23</t>
-  </si>
-  <si>
-    <t>pack24</t>
-  </si>
-  <si>
-    <t>pack25</t>
-  </si>
-  <si>
-    <t>pack26</t>
-  </si>
-  <si>
-    <t>pack27</t>
-  </si>
-  <si>
-    <t>pack28</t>
-  </si>
-  <si>
-    <t>pack29</t>
-  </si>
-  <si>
-    <t>pack30</t>
-  </si>
-  <si>
-    <t>pack31</t>
-  </si>
-  <si>
-    <t>pack32</t>
-  </si>
-  <si>
-    <t>pack33</t>
-  </si>
-  <si>
-    <t>pack34</t>
-  </si>
-  <si>
-    <t>pack35</t>
-  </si>
-  <si>
-    <t>pack36</t>
-  </si>
-  <si>
-    <t>pack37</t>
-  </si>
-  <si>
-    <t>pack38</t>
-  </si>
-  <si>
-    <t>pack39</t>
-  </si>
-  <si>
-    <t>pack40</t>
-  </si>
-  <si>
-    <t>pack41</t>
-  </si>
-  <si>
-    <t>pack42</t>
-  </si>
-  <si>
-    <t>pack43</t>
-  </si>
-  <si>
-    <t>pack44</t>
-  </si>
-  <si>
-    <t>pack45</t>
-  </si>
-  <si>
-    <t>pack46</t>
-  </si>
-  <si>
-    <t>pack47</t>
-  </si>
-  <si>
-    <t>pack48</t>
-  </si>
-  <si>
-    <t>pack49</t>
-  </si>
-  <si>
-    <t>pack50</t>
-  </si>
-  <si>
-    <t>pack51</t>
-  </si>
-  <si>
-    <t>pack52</t>
-  </si>
-  <si>
-    <t>pack53</t>
-  </si>
-  <si>
-    <t>pack54</t>
-  </si>
-  <si>
-    <t>pack55</t>
-  </si>
-  <si>
-    <t>pack56</t>
-  </si>
-  <si>
-    <t>pack57</t>
-  </si>
-  <si>
-    <t>pack58</t>
-  </si>
-  <si>
-    <t>pack59</t>
-  </si>
-  <si>
-    <t>pack60</t>
-  </si>
-  <si>
-    <t>pack61</t>
-  </si>
-  <si>
-    <t>pack62</t>
-  </si>
-  <si>
-    <t>pack63</t>
-  </si>
-  <si>
-    <t>pack64</t>
-  </si>
-  <si>
-    <t>pack65</t>
-  </si>
-  <si>
-    <t>pack66</t>
-  </si>
-  <si>
-    <t>pack67</t>
-  </si>
-  <si>
-    <t>pack68</t>
-  </si>
-  <si>
-    <t>pack69</t>
-  </si>
-  <si>
-    <t>pack70</t>
-  </si>
-  <si>
-    <t>pack71</t>
-  </si>
-  <si>
-    <t>pack72</t>
-  </si>
-  <si>
-    <t>pack73</t>
-  </si>
-  <si>
-    <t>pack74</t>
-  </si>
-  <si>
-    <t>pack75</t>
-  </si>
-  <si>
-    <t>pack76</t>
-  </si>
-  <si>
-    <t>pack77</t>
-  </si>
-  <si>
-    <t>pack78</t>
-  </si>
-  <si>
-    <t>pack79</t>
-  </si>
-  <si>
-    <t>pack80</t>
-  </si>
-  <si>
-    <t>pack81</t>
-  </si>
-  <si>
-    <t>pack82</t>
-  </si>
-  <si>
-    <t>pack83</t>
-  </si>
-  <si>
-    <t>pack84</t>
-  </si>
-  <si>
-    <t>pack85</t>
-  </si>
-  <si>
-    <t>pack86</t>
-  </si>
-  <si>
-    <t>pack87</t>
-  </si>
-  <si>
-    <t>pack88</t>
-  </si>
-  <si>
-    <t>pack89</t>
-  </si>
-  <si>
-    <t>pack90</t>
-  </si>
-  <si>
-    <t>pack91</t>
-  </si>
-  <si>
-    <t>pack92</t>
-  </si>
-  <si>
-    <t>pack93</t>
-  </si>
-  <si>
-    <t>pack94</t>
-  </si>
-  <si>
-    <t>pack95</t>
-  </si>
-  <si>
-    <t>pack96</t>
   </si>
 </sst>
 </file>
@@ -1116,32 +828,32 @@
       <selection activeCell="AN7" sqref="AN7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="24" customWidth="1"/>
-    <col min="35" max="35" width="23.42578125" customWidth="1"/>
-    <col min="36" max="36" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.28515625" customWidth="1"/>
+    <col min="35" max="35" width="23.5" customWidth="1"/>
+    <col min="36" max="36" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -1263,7 +975,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1385,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1507,7 +1219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1578,7 +1290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1700,7 +1412,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1822,7 +1534,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1890,7 +1602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2009,7 +1721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2128,7 +1840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2196,7 +1908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2315,7 +2027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2434,7 +2146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2502,7 +2214,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2621,7 +2333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2740,7 +2452,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2808,7 +2520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2876,7 +2588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2995,7 +2707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3114,7 +2826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3182,7 +2894,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3301,7 +3013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3417,7 +3129,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3482,7 +3194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3598,7 +3310,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3714,7 +3426,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3779,7 +3491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3895,7 +3607,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4011,7 +3723,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4076,7 +3788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4192,7 +3904,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4308,7 +4020,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4373,7 +4085,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4489,7 +4201,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4605,7 +4317,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4670,7 +4382,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4735,7 +4447,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4851,7 +4563,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4967,7 +4679,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5177,9 +4889,9 @@
       <selection activeCell="A7" sqref="A7:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5187,7 +4899,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5195,7 +4907,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5203,7 +4915,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -5211,7 +4923,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5219,7 +4931,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5239,18 +4951,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5261,7 +4973,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -5272,7 +4984,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -5280,489 +4992,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -5783,14 +5015,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5801,7 +5033,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -5812,7 +5044,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -5838,18 +5070,18 @@
       <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5896,7 +5128,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5916,7 +5148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5939,7 +5171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5959,7 +5191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5979,7 +5211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5999,7 +5231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -6019,7 +5251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -6039,7 +5271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -6059,7 +5291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -6076,7 +5308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -6093,7 +5325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -6113,7 +5345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -6133,7 +5365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -6150,7 +5382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -6170,7 +5402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -6187,7 +5419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -6210,7 +5442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -6230,7 +5462,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -6247,7 +5479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -6267,7 +5499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -6287,7 +5519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -6304,7 +5536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -6324,7 +5556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -6341,7 +5573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -6364,7 +5596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -6387,7 +5619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -6404,7 +5636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -6421,7 +5653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -6447,7 +5679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -6473,7 +5705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -6496,7 +5728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -6516,7 +5748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -6536,7 +5768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -6553,7 +5785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -6570,7 +5802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -6587,7 +5819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -6610,7 +5842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -6630,7 +5862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -6650,7 +5882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -6670,7 +5902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -6690,7 +5922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -6710,7 +5942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
Revert "revert with chao branch"
This reverts commit d4da21ad983d3a3751d639cce2436504250d4e4f.

Revert "revert merge with chao branch"

This reverts commit 38d97c2c49638c63accdaf27571bee5efe694066.

Revert "revert merge with chao branch"

This reverts commit bc4ac597a66cdc6b4b46c8f3043f173c7df6f23f.

Revert "revert merge with chao branch"

This reverts commit 44a53812a7b1db6d38b123a9832e12b8ced9f068.

Revert "revert merge with chao branch"

This reverts commit f6f792b2d7a0c6af6b8ec6f233dca2f5a8890351.

Revert "revert merge with chao branch"

This reverts commit 109f954ea2091b12b6b69514a606b9b87a48233e.
</commit_message>
<xml_diff>
--- a/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17740" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="239">
   <si>
     <t>text</t>
   </si>
@@ -452,6 +452,294 @@
   </si>
   <si>
     <t>org</t>
+  </si>
+  <si>
+    <t>pack1</t>
+  </si>
+  <si>
+    <t>pack2</t>
+  </si>
+  <si>
+    <t>pack3</t>
+  </si>
+  <si>
+    <t>pack4</t>
+  </si>
+  <si>
+    <t>pack5</t>
+  </si>
+  <si>
+    <t>pack6</t>
+  </si>
+  <si>
+    <t>pack7</t>
+  </si>
+  <si>
+    <t>pack8</t>
+  </si>
+  <si>
+    <t>pack9</t>
+  </si>
+  <si>
+    <t>pack10</t>
+  </si>
+  <si>
+    <t>pack11</t>
+  </si>
+  <si>
+    <t>pack12</t>
+  </si>
+  <si>
+    <t>pack13</t>
+  </si>
+  <si>
+    <t>pack14</t>
+  </si>
+  <si>
+    <t>pack15</t>
+  </si>
+  <si>
+    <t>pack16</t>
+  </si>
+  <si>
+    <t>pack17</t>
+  </si>
+  <si>
+    <t>pack18</t>
+  </si>
+  <si>
+    <t>pack19</t>
+  </si>
+  <si>
+    <t>pack20</t>
+  </si>
+  <si>
+    <t>pack21</t>
+  </si>
+  <si>
+    <t>pack22</t>
+  </si>
+  <si>
+    <t>pack23</t>
+  </si>
+  <si>
+    <t>pack24</t>
+  </si>
+  <si>
+    <t>pack25</t>
+  </si>
+  <si>
+    <t>pack26</t>
+  </si>
+  <si>
+    <t>pack27</t>
+  </si>
+  <si>
+    <t>pack28</t>
+  </si>
+  <si>
+    <t>pack29</t>
+  </si>
+  <si>
+    <t>pack30</t>
+  </si>
+  <si>
+    <t>pack31</t>
+  </si>
+  <si>
+    <t>pack32</t>
+  </si>
+  <si>
+    <t>pack33</t>
+  </si>
+  <si>
+    <t>pack34</t>
+  </si>
+  <si>
+    <t>pack35</t>
+  </si>
+  <si>
+    <t>pack36</t>
+  </si>
+  <si>
+    <t>pack37</t>
+  </si>
+  <si>
+    <t>pack38</t>
+  </si>
+  <si>
+    <t>pack39</t>
+  </si>
+  <si>
+    <t>pack40</t>
+  </si>
+  <si>
+    <t>pack41</t>
+  </si>
+  <si>
+    <t>pack42</t>
+  </si>
+  <si>
+    <t>pack43</t>
+  </si>
+  <si>
+    <t>pack44</t>
+  </si>
+  <si>
+    <t>pack45</t>
+  </si>
+  <si>
+    <t>pack46</t>
+  </si>
+  <si>
+    <t>pack47</t>
+  </si>
+  <si>
+    <t>pack48</t>
+  </si>
+  <si>
+    <t>pack49</t>
+  </si>
+  <si>
+    <t>pack50</t>
+  </si>
+  <si>
+    <t>pack51</t>
+  </si>
+  <si>
+    <t>pack52</t>
+  </si>
+  <si>
+    <t>pack53</t>
+  </si>
+  <si>
+    <t>pack54</t>
+  </si>
+  <si>
+    <t>pack55</t>
+  </si>
+  <si>
+    <t>pack56</t>
+  </si>
+  <si>
+    <t>pack57</t>
+  </si>
+  <si>
+    <t>pack58</t>
+  </si>
+  <si>
+    <t>pack59</t>
+  </si>
+  <si>
+    <t>pack60</t>
+  </si>
+  <si>
+    <t>pack61</t>
+  </si>
+  <si>
+    <t>pack62</t>
+  </si>
+  <si>
+    <t>pack63</t>
+  </si>
+  <si>
+    <t>pack64</t>
+  </si>
+  <si>
+    <t>pack65</t>
+  </si>
+  <si>
+    <t>pack66</t>
+  </si>
+  <si>
+    <t>pack67</t>
+  </si>
+  <si>
+    <t>pack68</t>
+  </si>
+  <si>
+    <t>pack69</t>
+  </si>
+  <si>
+    <t>pack70</t>
+  </si>
+  <si>
+    <t>pack71</t>
+  </si>
+  <si>
+    <t>pack72</t>
+  </si>
+  <si>
+    <t>pack73</t>
+  </si>
+  <si>
+    <t>pack74</t>
+  </si>
+  <si>
+    <t>pack75</t>
+  </si>
+  <si>
+    <t>pack76</t>
+  </si>
+  <si>
+    <t>pack77</t>
+  </si>
+  <si>
+    <t>pack78</t>
+  </si>
+  <si>
+    <t>pack79</t>
+  </si>
+  <si>
+    <t>pack80</t>
+  </si>
+  <si>
+    <t>pack81</t>
+  </si>
+  <si>
+    <t>pack82</t>
+  </si>
+  <si>
+    <t>pack83</t>
+  </si>
+  <si>
+    <t>pack84</t>
+  </si>
+  <si>
+    <t>pack85</t>
+  </si>
+  <si>
+    <t>pack86</t>
+  </si>
+  <si>
+    <t>pack87</t>
+  </si>
+  <si>
+    <t>pack88</t>
+  </si>
+  <si>
+    <t>pack89</t>
+  </si>
+  <si>
+    <t>pack90</t>
+  </si>
+  <si>
+    <t>pack91</t>
+  </si>
+  <si>
+    <t>pack92</t>
+  </si>
+  <si>
+    <t>pack93</t>
+  </si>
+  <si>
+    <t>pack94</t>
+  </si>
+  <si>
+    <t>pack95</t>
+  </si>
+  <si>
+    <t>pack96</t>
   </si>
 </sst>
 </file>
@@ -828,32 +1116,32 @@
       <selection activeCell="AN7" sqref="AN7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="24" customWidth="1"/>
-    <col min="35" max="35" width="23.5" customWidth="1"/>
-    <col min="36" max="36" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.33203125" customWidth="1"/>
+    <col min="35" max="35" width="23.42578125" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -975,7 +1263,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1097,7 +1385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1219,7 +1507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1290,7 +1578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1412,7 +1700,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1534,7 +1822,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1602,7 +1890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1721,7 +2009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1840,7 +2128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1908,7 +2196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2027,7 +2315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2146,7 +2434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2214,7 +2502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2333,7 +2621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2452,7 +2740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2520,7 +2808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2588,7 +2876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2707,7 +2995,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2826,7 +3114,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2894,7 +3182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3013,7 +3301,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3129,7 +3417,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3194,7 +3482,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3310,7 +3598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3426,7 +3714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3491,7 +3779,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3607,7 +3895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3723,7 +4011,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:39">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3788,7 +4076,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:39">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3904,7 +4192,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:39">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4020,7 +4308,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:39">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4085,7 +4373,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4201,7 +4489,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4317,7 +4605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4382,7 +4670,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4447,7 +4735,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4563,7 +4851,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4679,7 +4967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4889,9 +5177,9 @@
       <selection activeCell="A7" sqref="A7:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4899,7 +5187,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4907,7 +5195,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4915,7 +5203,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4923,7 +5211,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -4931,7 +5219,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -4951,18 +5239,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -4973,7 +5261,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -4984,7 +5272,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -4992,9 +5280,489 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -5015,14 +5783,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5033,7 +5801,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -5044,7 +5812,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -5070,18 +5838,18 @@
       <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5128,7 +5896,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5148,7 +5916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5171,7 +5939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5191,7 +5959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5211,7 +5979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5231,7 +5999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -5251,7 +6019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -5271,7 +6039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -5291,7 +6059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -5308,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -5325,7 +6093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -5345,7 +6113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -5365,7 +6133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -5382,7 +6150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -5402,7 +6170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5419,7 +6187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -5442,7 +6210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -5462,7 +6230,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -5479,7 +6247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -5499,7 +6267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -5519,7 +6287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -5536,7 +6304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -5556,7 +6324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -5573,7 +6341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -5596,7 +6364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -5619,7 +6387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -5636,7 +6404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -5653,7 +6421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -5679,7 +6447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -5705,7 +6473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -5728,7 +6496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -5748,7 +6516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -5768,7 +6536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -5785,7 +6553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -5802,7 +6570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -5819,7 +6587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -5842,7 +6610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -5862,7 +6630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -5882,7 +6650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -5902,7 +6670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -5922,7 +6690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -5942,7 +6710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
add only meta data test dataset
change interface of the entityMetaData to have all functionality of
defaultEntityMetaData

packages without parent or entity can be added to the packages table
</commit_message>
<xml_diff>
--- a/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app-omx/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17740" activeTab="2"/>
+    <workbookView xWindow="1760" yWindow="1300" windowWidth="25600" windowHeight="17740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="147">
   <si>
     <t>text</t>
   </si>
@@ -452,6 +452,18 @@
   </si>
   <si>
     <t>org</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>euro</t>
+  </si>
+  <si>
+    <t>earth</t>
+  </si>
+  <si>
+    <t>universe</t>
   </si>
 </sst>
 </file>
@@ -4951,10 +4963,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4995,6 +5007,32 @@
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>